<commit_message>
First implementation of DAB
First tries to implement DAB in PyPowerSim.
</commit_message>
<xml_diff>
--- a/para/Swi/IAUT300N10S5N015.xlsx
+++ b/para/Swi/IAUT300N10S5N015.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f215465b21b5e6e2/Studium/34_Github/PyPowerSim/para/Swi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1695" documentId="11_AD4DB114E441178AC67DF439BED5CE16693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4714ED8-1478-487D-897D-B8B97C6FFD3E}"/>
+  <xr:revisionPtr revIDLastSave="1700" documentId="11_AD4DB114E441178AC67DF439BED5CE16693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351CA075-42DD-4AE8-9673-4A248FCEE881}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -937,6 +937,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,15 +953,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2337,6 +2337,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2344,7 +2345,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2449,7 +2449,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2898,6 +2898,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2905,7 +2906,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3098,6 +3098,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3191,6 +3215,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4257,6 +4305,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4264,7 +4313,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4457,6 +4505,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4550,6 +4622,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5616,6 +5712,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -5623,7 +5720,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5816,6 +5912,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5909,6 +6029,30 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6975,6 +7119,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -6982,7 +7127,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8382,6 +8526,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -8389,7 +8534,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -9789,6 +9933,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -9796,7 +9941,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -11196,6 +11340,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -11203,7 +11348,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -12603,6 +12747,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -12610,7 +12755,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -12715,7 +12859,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13378,6 +13522,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -13385,7 +13530,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -19364,10 +19508,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -19634,7 +19774,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19755,8 +19895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCB0370-656A-4BCA-B950-AA707D31C9FC}">
   <dimension ref="A1:AA184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D15"/>
+    <sheetView tabSelected="1" topLeftCell="G25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20627,36 +20767,36 @@
     </row>
     <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="45"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="42"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
     </row>
     <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="32"/>
@@ -20909,36 +21049,36 @@
     </row>
     <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="45"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="42"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="42"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="45"/>
     </row>
     <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33"/>
@@ -20988,8 +21128,12 @@
         <f>F$16</f>
         <v>0</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
+      <c r="B55" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C55" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
@@ -21004,8 +21148,12 @@
         <f>G$16</f>
         <v>1</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
+      <c r="B56" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C56" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -21020,8 +21168,12 @@
         <f>H$16</f>
         <v>5</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+      <c r="B57" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C57" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
@@ -21036,8 +21188,12 @@
         <f>I$16</f>
         <v>10</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
+      <c r="B58" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C58" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
@@ -21052,8 +21208,12 @@
         <f>J$16</f>
         <v>20</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
+      <c r="B59" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C59" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
@@ -21068,8 +21228,12 @@
         <f>K$16</f>
         <v>50</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
+      <c r="B60" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C60" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -21084,8 +21248,12 @@
         <f>L$16</f>
         <v>100</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C61" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
@@ -21100,8 +21268,12 @@
         <f>M$16</f>
         <v>300</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
+      <c r="B62" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C62" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D62" s="17"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
@@ -21145,36 +21317,36 @@
     </row>
     <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="44"/>
-      <c r="J72" s="44"/>
-      <c r="K72" s="45"/>
+      <c r="B72" s="41"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="41"/>
+      <c r="K72" s="42"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="41"/>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="41"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="41"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="42"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="45"/>
     </row>
     <row r="74" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="34"/>
@@ -21224,8 +21396,12 @@
         <f>F$16</f>
         <v>0</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
+      <c r="B75" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C75" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
@@ -21240,8 +21416,12 @@
         <f>G$16</f>
         <v>1</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
+      <c r="B76" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C76" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
       <c r="F76" s="17"/>
@@ -21256,8 +21436,12 @@
         <f>H$16</f>
         <v>5</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
+      <c r="B77" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C77" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
@@ -21272,8 +21456,12 @@
         <f>I$16</f>
         <v>10</v>
       </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
+      <c r="B78" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C78" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
       <c r="F78" s="17"/>
@@ -21288,8 +21476,12 @@
         <f>J$16</f>
         <v>20</v>
       </c>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
+      <c r="B79" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C79" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
       <c r="F79" s="17"/>
@@ -21304,8 +21496,12 @@
         <f>K$16</f>
         <v>50</v>
       </c>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
+      <c r="B80" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C80" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
       <c r="F80" s="17"/>
@@ -21320,8 +21516,12 @@
         <f>L$16</f>
         <v>100</v>
       </c>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
+      <c r="B81" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C81" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D81" s="17"/>
       <c r="E81" s="17"/>
       <c r="F81" s="17"/>
@@ -21336,8 +21536,12 @@
         <f>M$16</f>
         <v>300</v>
       </c>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
+      <c r="B82" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C82" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D82" s="17"/>
       <c r="E82" s="17"/>
       <c r="F82" s="17"/>
@@ -21381,36 +21585,36 @@
     </row>
     <row r="91" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="43" t="s">
+      <c r="A92" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B92" s="44"/>
-      <c r="C92" s="44"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="44"/>
-      <c r="I92" s="44"/>
-      <c r="J92" s="44"/>
-      <c r="K92" s="45"/>
+      <c r="B92" s="41"/>
+      <c r="C92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="41"/>
+      <c r="K92" s="42"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C93" s="41"/>
-      <c r="D93" s="41"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="41"/>
-      <c r="G93" s="41"/>
-      <c r="H93" s="41"/>
-      <c r="I93" s="41"/>
-      <c r="J93" s="41"/>
-      <c r="K93" s="42"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="44"/>
+      <c r="K93" s="45"/>
     </row>
     <row r="94" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="32"/>
@@ -21460,8 +21664,12 @@
         <f>F$17</f>
         <v>0</v>
       </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
+      <c r="B95" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C95" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D95" s="17"/>
       <c r="E95" s="17"/>
       <c r="F95" s="17"/>
@@ -21476,8 +21684,12 @@
         <f>G$17</f>
         <v>1</v>
       </c>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
+      <c r="B96" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C96" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D96" s="17"/>
       <c r="E96" s="17"/>
       <c r="F96" s="17"/>
@@ -21492,8 +21704,12 @@
         <f>H$17</f>
         <v>5</v>
       </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
+      <c r="B97" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C97" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D97" s="17"/>
       <c r="E97" s="17"/>
       <c r="F97" s="17"/>
@@ -21508,8 +21724,12 @@
         <f>I$17</f>
         <v>10</v>
       </c>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
+      <c r="B98" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C98" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D98" s="17"/>
       <c r="E98" s="17"/>
       <c r="F98" s="17"/>
@@ -21524,8 +21744,12 @@
         <f>J$17</f>
         <v>20</v>
       </c>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
+      <c r="B99" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C99" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D99" s="17"/>
       <c r="E99" s="17"/>
       <c r="F99" s="17"/>
@@ -21540,8 +21764,12 @@
         <f>K$17</f>
         <v>50</v>
       </c>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
+      <c r="B100" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C100" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D100" s="17"/>
       <c r="E100" s="17"/>
       <c r="F100" s="17"/>
@@ -21556,8 +21784,12 @@
         <f>L$17</f>
         <v>100</v>
       </c>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
+      <c r="B101" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C101" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
       <c r="F101" s="17"/>
@@ -21572,8 +21804,12 @@
         <f>M$17</f>
         <v>300</v>
       </c>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
+      <c r="B102" s="17">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C102" s="17">
+        <v>1.1999999999999999E-6</v>
+      </c>
       <c r="D102" s="17"/>
       <c r="E102" s="17"/>
       <c r="F102" s="17"/>
@@ -21617,37 +21853,37 @@
     </row>
     <row r="111" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A112" s="43" t="s">
+      <c r="A112" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B112" s="44"/>
-      <c r="C112" s="44"/>
-      <c r="D112" s="44"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="44"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="44"/>
-      <c r="I112" s="44"/>
-      <c r="J112" s="44"/>
-      <c r="K112" s="45"/>
+      <c r="B112" s="41"/>
+      <c r="C112" s="41"/>
+      <c r="D112" s="41"/>
+      <c r="E112" s="41"/>
+      <c r="F112" s="41"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="41"/>
+      <c r="I112" s="41"/>
+      <c r="J112" s="41"/>
+      <c r="K112" s="42"/>
       <c r="L112" s="2"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C113" s="41"/>
-      <c r="D113" s="41"/>
-      <c r="E113" s="41"/>
-      <c r="F113" s="41"/>
-      <c r="G113" s="41"/>
-      <c r="H113" s="41"/>
-      <c r="I113" s="41"/>
-      <c r="J113" s="41"/>
-      <c r="K113" s="42"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="45"/>
       <c r="L113" s="1"/>
     </row>
     <row r="114" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -21898,36 +22134,36 @@
     </row>
     <row r="131" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A132" s="43" t="s">
+      <c r="A132" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="B132" s="44"/>
-      <c r="C132" s="44"/>
-      <c r="D132" s="44"/>
-      <c r="E132" s="44"/>
-      <c r="F132" s="44"/>
-      <c r="G132" s="44"/>
-      <c r="H132" s="44"/>
-      <c r="I132" s="44"/>
-      <c r="J132" s="44"/>
-      <c r="K132" s="45"/>
+      <c r="B132" s="41"/>
+      <c r="C132" s="41"/>
+      <c r="D132" s="41"/>
+      <c r="E132" s="41"/>
+      <c r="F132" s="41"/>
+      <c r="G132" s="41"/>
+      <c r="H132" s="41"/>
+      <c r="I132" s="41"/>
+      <c r="J132" s="41"/>
+      <c r="K132" s="42"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B133" s="40" t="s">
+      <c r="B133" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C133" s="41"/>
-      <c r="D133" s="41"/>
-      <c r="E133" s="41"/>
-      <c r="F133" s="41"/>
-      <c r="G133" s="41"/>
-      <c r="H133" s="41"/>
-      <c r="I133" s="41"/>
-      <c r="J133" s="41"/>
-      <c r="K133" s="42"/>
+      <c r="C133" s="44"/>
+      <c r="D133" s="44"/>
+      <c r="E133" s="44"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="44"/>
+      <c r="H133" s="44"/>
+      <c r="I133" s="44"/>
+      <c r="J133" s="44"/>
+      <c r="K133" s="45"/>
     </row>
     <row r="134" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="32"/>
@@ -22166,36 +22402,36 @@
     </row>
     <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A152" s="43" t="s">
+      <c r="A152" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="B152" s="44"/>
-      <c r="C152" s="44"/>
-      <c r="D152" s="44"/>
-      <c r="E152" s="44"/>
-      <c r="F152" s="44"/>
-      <c r="G152" s="44"/>
-      <c r="H152" s="44"/>
-      <c r="I152" s="44"/>
-      <c r="J152" s="44"/>
-      <c r="K152" s="45"/>
+      <c r="B152" s="41"/>
+      <c r="C152" s="41"/>
+      <c r="D152" s="41"/>
+      <c r="E152" s="41"/>
+      <c r="F152" s="41"/>
+      <c r="G152" s="41"/>
+      <c r="H152" s="41"/>
+      <c r="I152" s="41"/>
+      <c r="J152" s="41"/>
+      <c r="K152" s="42"/>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B153" s="40" t="s">
+      <c r="B153" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C153" s="41"/>
-      <c r="D153" s="41"/>
-      <c r="E153" s="41"/>
-      <c r="F153" s="41"/>
-      <c r="G153" s="41"/>
-      <c r="H153" s="41"/>
-      <c r="I153" s="41"/>
-      <c r="J153" s="41"/>
-      <c r="K153" s="42"/>
+      <c r="C153" s="44"/>
+      <c r="D153" s="44"/>
+      <c r="E153" s="44"/>
+      <c r="F153" s="44"/>
+      <c r="G153" s="44"/>
+      <c r="H153" s="44"/>
+      <c r="I153" s="44"/>
+      <c r="J153" s="44"/>
+      <c r="K153" s="45"/>
     </row>
     <row r="154" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="32"/>
@@ -22434,36 +22670,36 @@
     </row>
     <row r="171" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A172" s="43" t="s">
+      <c r="A172" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="B172" s="44"/>
-      <c r="C172" s="44"/>
-      <c r="D172" s="44"/>
-      <c r="E172" s="44"/>
-      <c r="F172" s="44"/>
-      <c r="G172" s="44"/>
-      <c r="H172" s="44"/>
-      <c r="I172" s="44"/>
-      <c r="J172" s="44"/>
-      <c r="K172" s="45"/>
+      <c r="B172" s="41"/>
+      <c r="C172" s="41"/>
+      <c r="D172" s="41"/>
+      <c r="E172" s="41"/>
+      <c r="F172" s="41"/>
+      <c r="G172" s="41"/>
+      <c r="H172" s="41"/>
+      <c r="I172" s="41"/>
+      <c r="J172" s="41"/>
+      <c r="K172" s="42"/>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B173" s="40" t="s">
+      <c r="B173" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C173" s="41"/>
-      <c r="D173" s="41"/>
-      <c r="E173" s="41"/>
-      <c r="F173" s="41"/>
-      <c r="G173" s="41"/>
-      <c r="H173" s="41"/>
-      <c r="I173" s="41"/>
-      <c r="J173" s="41"/>
-      <c r="K173" s="42"/>
+      <c r="C173" s="44"/>
+      <c r="D173" s="44"/>
+      <c r="E173" s="44"/>
+      <c r="F173" s="44"/>
+      <c r="G173" s="44"/>
+      <c r="H173" s="44"/>
+      <c r="I173" s="44"/>
+      <c r="J173" s="44"/>
+      <c r="K173" s="45"/>
     </row>
     <row r="174" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="32"/>
@@ -22702,22 +22938,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B73:K73"/>
+    <mergeCell ref="A92:K92"/>
+    <mergeCell ref="B93:K93"/>
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="B113:K113"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="B53:K53"/>
+    <mergeCell ref="A72:K72"/>
     <mergeCell ref="A152:K152"/>
     <mergeCell ref="B153:K153"/>
     <mergeCell ref="A172:K172"/>
     <mergeCell ref="B173:K173"/>
     <mergeCell ref="A132:K132"/>
     <mergeCell ref="B133:K133"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="B53:K53"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="B73:K73"/>
-    <mergeCell ref="A92:K92"/>
-    <mergeCell ref="B93:K93"/>
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="B113:K113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>